<commit_message>
udah cek template word
</commit_message>
<xml_diff>
--- a/src/sample/template/Surat Keterangan Bepergian.xlsx
+++ b/src/sample/template/Surat Keterangan Bepergian.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="18">
   <si>
     <t>Nomor Surat</t>
   </si>
@@ -436,7 +436,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A433DDF2-FF8B-45BF-AE81-BFD2B49E48CB}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
@@ -541,6 +541,59 @@
         <v>16</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>